<commit_message>
Update JSON range function and host files
</commit_message>
<xml_diff>
--- a/docs/examples/test2.xlsx
+++ b/docs/examples/test2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abhis\Documents\Github Projects\Server\excel-stream\example-excel-addin\export\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{143BA111-F8CB-4717-8578-43F603CDE10B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB07831-694F-4646-BD59-DA5D08CDFF95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -917,7 +917,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="" visibility="1" width="700" row="3">
+  <wetp:taskpane dockstate="" visibility="1" width="700" row="2">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -931,11 +931,15 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions val="1"/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_STREAM_SUBSCRIBE</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_STREAM_FETCHJSON</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_STREAM_EXTRACT</we:customFunctionIds>
+        <we:customFunctionIds>_xldudf_STREAM_PARSEJSONRANGE</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_STREAM_GETSTARCOUNT</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_STREAM_CLOCK</we:customFunctionIds>
         <we:customFunctionIds>_xldudf_STREAM_INCREMENT</we:customFunctionIds>
@@ -952,7 +956,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -978,84 +982,46 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="str" cm="1">
-        <f t="array" ref="A5:L6">_xldudf_STREAM_PARSEJSONRANGE(A3)</f>
-        <v>ticker</v>
+        <f t="array" ref="A5:L5">_xldudf_STREAM_PARSEJSONRANGE(A3)</f>
+        <v>ACE.AX</v>
       </c>
       <c r="B5" t="str">
-        <v>companyshortname</v>
+        <v>Acusensus Ltd</v>
       </c>
       <c r="C5" t="str">
-        <v>exchange_short_name</v>
+        <v>ASX</v>
       </c>
       <c r="D5" t="str">
-        <v>filingdate</v>
-      </c>
-      <c r="E5" t="str">
-        <v>startdatetime</v>
+        <v>2022-10-23T04:00:00.000Z</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
       </c>
       <c r="F5" t="str">
-        <v>amendeddate</v>
-      </c>
-      <c r="G5" t="str">
-        <v>pricefrom</v>
-      </c>
-      <c r="H5" t="str">
-        <v>priceto</v>
-      </c>
-      <c r="I5" t="str">
-        <v>offerprice</v>
+        <v>2022-12-06T05:00:00.000Z</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>4</v>
       </c>
       <c r="J5" t="str">
-        <v>currencyname</v>
-      </c>
-      <c r="K5" t="str">
-        <v>shares</v>
+        <v>AUD</v>
+      </c>
+      <c r="K5">
+        <v>5000000</v>
       </c>
       <c r="L5" t="str">
-        <v>dealtype</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A6" t="str">
-        <v>ACE.AX</v>
-      </c>
-      <c r="B6" t="str">
-        <v>Acusensus Ltd</v>
-      </c>
-      <c r="C6" t="str">
-        <v>ASX</v>
-      </c>
-      <c r="D6" t="str">
-        <v>2022-10-23T04:00:00.000Z</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" t="str">
-        <v>2022-12-06T05:00:00.000Z</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>4</v>
-      </c>
-      <c r="J6" t="str">
-        <v>AUD</v>
-      </c>
-      <c r="K6">
-        <v>5000000</v>
-      </c>
-      <c r="L6" t="str">
         <v>Amended</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" t="str" cm="1">
-        <f t="array" ref="A10:L12">_xldudf_STREAM_PARSEJSONRANGE(_xldudf_STREAM_EXTRACT(A1, "data"))</f>
+        <f t="array" ref="A10:L12">_xldudf_STREAM_PARSEJSONRANGE(_xldudf_STREAM_EXTRACT(A1, "data"), TRUE)</f>
         <v>ticker</v>
       </c>
       <c r="B10" t="str">

</xml_diff>